<commit_message>
final update before friday
</commit_message>
<xml_diff>
--- a/data/canadaTextParsing/Committees/raw_canada_subcommittees.xlsx
+++ b/data/canadaTextParsing/Committees/raw_canada_subcommittees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luzhang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luzhang/Documents/GitHub/CompLegFall2019/data/canadaTextParsing/Committees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE67967B-3754-FD4F-A0ED-DFA3C0CA11DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1846B906-FFED-CC4B-8FEC-6D8A06DF0FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{1DE95D9F-98D0-7548-A8BD-F8D0C8A4D8E7}"/>
+    <workbookView xWindow="5020" yWindow="460" windowWidth="21220" windowHeight="16420" xr2:uid="{1DE95D9F-98D0-7548-A8BD-F8D0C8A4D8E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="141">
   <si>
     <t>parliament_number</t>
   </si>
@@ -445,6 +445,15 @@
   </si>
   <si>
     <t>SCC3</t>
+  </si>
+  <si>
+    <t>SBIL</t>
+  </si>
+  <si>
+    <t>SLIB</t>
+  </si>
+  <si>
+    <t>Subcommittee of LIBI on Committee Budgets</t>
   </si>
 </sst>
 </file>
@@ -810,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0195B6-623E-F848-8507-974D8577F5D0}">
   <dimension ref="A1:G233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G234" sqref="G234"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="E243" sqref="E243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3392,7 +3401,7 @@
         <v>40628</v>
       </c>
       <c r="E112" t="s">
-        <v>65</v>
+        <v>138</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>89</v>
@@ -4036,7 +4045,7 @@
         <v>40177</v>
       </c>
       <c r="E140" t="s">
-        <v>65</v>
+        <v>138</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>89</v>
@@ -6152,10 +6161,10 @@
         <v>38685</v>
       </c>
       <c r="E232" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="F232" s="2" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="G232" t="s">
         <v>84</v>

</xml_diff>